<commit_message>
Enabled 1PSUPPORT service from testng.xml file
</commit_message>
<xml_diff>
--- a/src/test/test-data/SupportTestData.xlsx
+++ b/src/test/test-data/SupportTestData.xlsx
@@ -69,13 +69,13 @@
     <t>Verify that access token is returned successfully by using support API</t>
   </si>
   <si>
-    <t>status=200||access_token=00D3000000000un!AR8AQOHrSQ2MJFFU5D8EgAQ4ZfVUxJdKOstT4Iak4B5PULuBjpLU5JL5IT.j.1E1tuP3Ywl85ht70CnNrrPG2S1lo5LGNeJv||instance_url=https://na33.salesforce.com</t>
-  </si>
-  <si>
     <t>user_ip</t>
   </si>
   <si>
     <t>OPQA-5284</t>
+  </si>
+  <si>
+    <t>status=200||access_token=00D3000000000un!AR8AQC7cJ81UAeuz.9pdSgmblAlTzFyJzZpIiIOvRwg..r3e.y4142nomU4aNdk.xoIopCgcmPiZvQy8EHfsOPVwykB1_AKq||instance_url=https://na33.salesforce.com</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>15</v>
@@ -564,10 +564,10 @@
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed 1PSUPPORT failed APIs.
</commit_message>
<xml_diff>
--- a/src/test/test-data/SupportTestData.xlsx
+++ b/src/test/test-data/SupportTestData.xlsx
@@ -75,7 +75,7 @@
     <t>OPQA-5284</t>
   </si>
   <si>
-    <t>status=200||access_token=00D3000000000un!AR8AQC7cJ81UAeuz.9pdSgmblAlTzFyJzZpIiIOvRwg..r3e.y4142nomU4aNdk.xoIopCgcmPiZvQy8EHfsOPVwykB1_AKq||instance_url=https://na33.salesforce.com</t>
+    <t>status=200||instance_url=https://na33.salesforce.com</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Disabled IPA from autorun in testng.xml, Fixed support failed tests.
</commit_message>
<xml_diff>
--- a/src/test/test-data/SupportTestData.xlsx
+++ b/src/test/test-data/SupportTestData.xlsx
@@ -75,7 +75,7 @@
     <t>OPQA-5284</t>
   </si>
   <si>
-    <t>status=200||instance_url=https://na33.salesforce.com</t>
+    <t>status=200</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>